<commit_message>
actualziar los codigos y xlsx de muestra
</commit_message>
<xml_diff>
--- a/Prueba10_con_creditos.xlsx
+++ b/Prueba10_con_creditos.xlsx
@@ -629,10 +629,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
       <c r="H4" t="n">
         <v>3.9</v>
       </c>
@@ -791,10 +793,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
       <c r="H7" t="n">
         <v>3.7</v>
       </c>
@@ -845,10 +849,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
       <c r="H8" t="n">
         <v>3.7</v>
       </c>
@@ -899,10 +905,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
       <c r="H9" t="n">
         <v>4</v>
       </c>
@@ -1007,10 +1015,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>2</v>
+      </c>
       <c r="H11" t="n">
         <v>3.5</v>
       </c>
@@ -1169,10 +1179,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
       <c r="H14" t="n">
         <v>4.1</v>
       </c>
@@ -1223,10 +1235,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>4</v>
+      </c>
       <c r="H15" t="n">
         <v>3.9</v>
       </c>
@@ -1601,10 +1615,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>2</v>
+      </c>
       <c r="H22" t="n">
         <v>3.2</v>
       </c>
@@ -1655,10 +1671,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>4</v>
+      </c>
       <c r="H23" t="n">
         <v>4.1</v>
       </c>
@@ -3923,10 +3941,12 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr"/>
+          <t>Nivelación</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>1</v>
+      </c>
       <c r="H65" t="n">
         <v>4</v>
       </c>
@@ -3977,10 +3997,12 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>1</v>
+      </c>
       <c r="H66" t="n">
         <v>3.6</v>
       </c>
@@ -4031,10 +4053,12 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr"/>
+          <t>Nivelación</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>1</v>
+      </c>
       <c r="H67" t="n">
         <v>3.4</v>
       </c>
@@ -4085,10 +4109,12 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>1</v>
+      </c>
       <c r="H68" t="n">
         <v>3</v>
       </c>
@@ -4193,10 +4219,12 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>1</v>
+      </c>
       <c r="H70" t="n">
         <v>3.8</v>
       </c>
@@ -4247,10 +4275,12 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>2</v>
+      </c>
       <c r="H71" t="n">
         <v>0</v>
       </c>
@@ -4301,10 +4331,12 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>1</v>
+      </c>
       <c r="H72" t="n">
         <v>3.5</v>
       </c>
@@ -4355,10 +4387,12 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>4</v>
+      </c>
       <c r="H73" t="n">
         <v>3.5</v>
       </c>
@@ -4409,10 +4443,12 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>2</v>
+      </c>
       <c r="H74" t="n">
         <v>2.5</v>
       </c>
@@ -4517,10 +4553,12 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>5</v>
+      </c>
       <c r="H76" t="n">
         <v>3.1</v>
       </c>
@@ -4571,10 +4609,12 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>3</v>
+      </c>
       <c r="H77" t="n">
         <v>3.7</v>
       </c>
@@ -4625,10 +4665,12 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>2</v>
+      </c>
       <c r="H78" t="n">
         <v>2.8</v>
       </c>
@@ -4679,10 +4721,12 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>2</v>
+      </c>
       <c r="H79" t="n">
         <v>3</v>
       </c>
@@ -4733,10 +4777,12 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>4</v>
+      </c>
       <c r="H80" t="n">
         <v>4.4</v>
       </c>
@@ -4841,10 +4887,12 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>3</v>
+      </c>
       <c r="H82" t="n">
         <v>3.1</v>
       </c>
@@ -4895,10 +4943,12 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>2</v>
+      </c>
       <c r="H83" t="n">
         <v>3.9</v>
       </c>
@@ -4949,10 +4999,12 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>3</v>
+      </c>
       <c r="H84" t="n">
         <v>4.3</v>
       </c>
@@ -5003,10 +5055,12 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>4</v>
+      </c>
       <c r="H85" t="n">
         <v>3.3</v>
       </c>
@@ -5057,10 +5111,12 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>3</v>
+      </c>
       <c r="H86" t="n">
         <v>3.3</v>
       </c>
@@ -5111,10 +5167,12 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>4</v>
+      </c>
       <c r="H87" t="n">
         <v>3.7</v>
       </c>
@@ -5165,10 +5223,12 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>3</v>
+      </c>
       <c r="H88" t="n">
         <v>3.8</v>
       </c>
@@ -5273,10 +5333,12 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>5</v>
+      </c>
       <c r="H90" t="n">
         <v>3.9</v>
       </c>
@@ -5327,10 +5389,12 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>4</v>
+      </c>
       <c r="H91" t="n">
         <v>4.6</v>
       </c>
@@ -5381,10 +5445,12 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>2</v>
+      </c>
       <c r="H92" t="n">
         <v>3.3</v>
       </c>
@@ -5435,10 +5501,12 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>6</v>
+      </c>
       <c r="H93" t="n">
         <v>3</v>
       </c>
@@ -5543,10 +5611,12 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>5</v>
+      </c>
       <c r="H95" t="n">
         <v>4</v>
       </c>
@@ -5651,10 +5721,12 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>4</v>
+      </c>
       <c r="H97" t="n">
         <v>3.7</v>
       </c>
@@ -5705,10 +5777,12 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>6</v>
+      </c>
       <c r="H98" t="n">
         <v>3.9</v>
       </c>
@@ -5759,10 +5833,12 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>7</v>
+      </c>
       <c r="H99" t="n">
         <v>3.6</v>
       </c>
@@ -5813,10 +5889,12 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>6</v>
+      </c>
       <c r="H100" t="n">
         <v>3.6</v>
       </c>
@@ -5867,10 +5945,12 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G101" t="n">
+        <v>5</v>
+      </c>
       <c r="H101" t="n">
         <v>3</v>
       </c>
@@ -5921,10 +6001,12 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>6</v>
+      </c>
       <c r="H102" t="n">
         <v>2.8</v>
       </c>
@@ -5975,10 +6057,12 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G103" t="n">
+        <v>6</v>
+      </c>
       <c r="H103" t="n">
         <v>3.2</v>
       </c>
@@ -6191,10 +6275,12 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>7</v>
+      </c>
       <c r="H107" t="n">
         <v>2.7</v>
       </c>
@@ -6245,10 +6331,12 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>7</v>
+      </c>
       <c r="H108" t="n">
         <v>3.4</v>
       </c>
@@ -6299,10 +6387,12 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G109" t="n">
+        <v>7</v>
+      </c>
       <c r="H109" t="n">
         <v>3</v>
       </c>
@@ -6407,10 +6497,12 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G111" t="n">
+        <v>7</v>
+      </c>
       <c r="H111" t="n">
         <v>3</v>
       </c>
@@ -6461,10 +6553,12 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G112" t="n">
+        <v>7</v>
+      </c>
       <c r="H112" t="n">
         <v>3</v>
       </c>
@@ -6515,10 +6609,12 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G113" t="n">
+        <v>8</v>
+      </c>
       <c r="H113" t="n">
         <v>3.5</v>
       </c>
@@ -6677,10 +6773,12 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G116" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G116" t="n">
+        <v>8</v>
+      </c>
       <c r="H116" t="n">
         <v>3.5</v>
       </c>
@@ -6731,10 +6829,12 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G117" t="n">
+        <v>5</v>
+      </c>
       <c r="H117" t="n">
         <v>3</v>
       </c>
@@ -6785,10 +6885,12 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G118" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G118" t="n">
+        <v>8</v>
+      </c>
       <c r="H118" t="n">
         <v>3.7</v>
       </c>
@@ -6839,10 +6941,12 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G119" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G119" t="n">
+        <v>9</v>
+      </c>
       <c r="H119" t="n">
         <v>3.7</v>
       </c>
@@ -6947,10 +7051,12 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G121" t="inlineStr"/>
+          <t>Optativa de Producción</t>
+        </is>
+      </c>
+      <c r="G121" t="n">
+        <v>9</v>
+      </c>
       <c r="H121" t="n">
         <v>0</v>
       </c>
@@ -7057,7 +7163,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Optativa de producción (C)</t>
+          <t>Optativa de Producción</t>
         </is>
       </c>
       <c r="G123" t="n">
@@ -7493,7 +7599,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Optativa de producción (C)</t>
+          <t>Optativa de Producción</t>
         </is>
       </c>
       <c r="G131" t="n">

</xml_diff>

<commit_message>
Correción de codigo para asegurar nombres correctos
</commit_message>
<xml_diff>
--- a/Prueba10_con_creditos.xlsx
+++ b/Prueba10_con_creditos.xlsx
@@ -4825,7 +4825,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Obligatoria (C) Laboratorio de química básica</t>
+          <t>Laboratorio de química básica</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -4833,10 +4833,12 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr"/>
+          <t>Fund. Obligatoria</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>2</v>
+      </c>
       <c r="H81" t="n">
         <v>3.6</v>
       </c>
@@ -5659,7 +5661,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Obligatoria (C) Entomología</t>
+          <t>Entomología</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -5667,10 +5669,12 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Libre Elección (L)</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr"/>
+          <t>Disciplinar</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>6</v>
+      </c>
       <c r="H96" t="n">
         <v>4.2</v>
       </c>

</xml_diff>

<commit_message>
Agregacion de Prerequisitos, calculo de cupos, adaptacion para coioncidencia por nombre o por codigo de asignatura
</commit_message>
<xml_diff>
--- a/Prueba10_con_creditos.xlsx
+++ b/Prueba10_con_creditos.xlsx
@@ -3971,7 +3971,7 @@
         </is>
       </c>
       <c r="G64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -4027,7 +4027,7 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>

</xml_diff>